<commit_message>
made a bash script to test all files and edited test_mkfiles to make it cleaner as well as fixing some minor issues with spaces for mk_sam_files
</commit_message>
<xml_diff>
--- a/sam_sample_template.xlsx
+++ b/sam_sample_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>site_info</t>
   </si>
@@ -32,10 +32,25 @@
     <t>elevation</t>
   </si>
   <si>
+    <t>---------------–------------------------------------------------------------------------------Sun Compass Information---------------------------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>---------------------------------------------------Calculated Fields----------------------------------------------------</t>
+  </si>
+  <si>
     <t>mag_dec</t>
   </si>
   <si>
-    <t>---------------–------------------------------------------------------------------------------Sun Compass Information-------------------------------------------------------------------------------------------</t>
+    <t>only used if no sun data</t>
+  </si>
+  <si>
+    <t>all sun compass info is optional</t>
+  </si>
+  <si>
+    <t>Optional Field</t>
+  </si>
+  <si>
+    <t>default core strike</t>
   </si>
   <si>
     <t>site_id</t>
@@ -108,7 +123,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -129,6 +144,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <color rgb="FF161616"/>
+      <name val="Noto Sans"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -192,7 +214,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -219,6 +241,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -234,6 +264,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF161616"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -244,8 +334,8 @@
   </sheetPr>
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P6" activeCellId="0" sqref="P6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q7" activeCellId="0" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -282,79 +372,94 @@
         <v>4</v>
       </c>
       <c r="B5" s="5"/>
+      <c r="G5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="G6" s="6" t="s">
-        <v>6</v>
+      <c r="E6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="7" t="s">
+      <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="B7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="C7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="D7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="E7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="F7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="G7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="H7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="I7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="J7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="K7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="Q7" s="7" t="s">
+      <c r="L7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="R7" s="7" t="s">
+      <c r="M7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="S7" s="7" t="s">
+      <c r="N7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="T7" s="7" t="s">
+      <c r="O7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="U7" s="7" t="s">
+      <c r="P7" s="9" t="s">
         <v>27</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="U7" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed error in finding directory and error in pd.readcsv reading columns as well as updating the spreadsheet template
</commit_message>
<xml_diff>
--- a/sam_sample_template.xlsx
+++ b/sam_sample_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>site_info</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>calculated_IGRF</t>
+  </si>
+  <si>
+    <t>IGRF_local_dec</t>
   </si>
   <si>
     <t>calculated_mag_dec</t>
@@ -212,7 +215,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -247,6 +250,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -329,7 +336,7 @@
   <dimension ref="1:6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U7" activeCellId="0" sqref="U7"/>
+      <selection pane="topLeft" activeCell="U11" activeCellId="0" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5547,13 +5554,15 @@
       <c r="S6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="T6" s="8" t="s">
+      <c r="T6" s="9" t="s">
         <v>30</v>
       </c>
       <c r="U6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="V6" s="0"/>
+      <c r="V6" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="W6" s="0"/>
       <c r="X6" s="0"/>
       <c r="Y6" s="0"/>

</xml_diff>

<commit_message>
mk_sam_file: fixed problem with different line breaks on different architectures, corrected bedding, made print outs more informative mk_sam_utilities: compiled all dependencies outside scipy and put them here deleted other files sam_sample_template: changed corrected bedding boolean name create_headers.sh: made bash script that allows header creation on a set of csvs quickly as long as they follow the current namming convention used by the lab
</commit_message>
<xml_diff>
--- a/sam_sample_template.xlsx
+++ b/sam_sample_template.xlsx
@@ -53,7 +53,7 @@
     <t>only used if no sun data</t>
   </si>
   <si>
-    <t>[default is no] (yes or no)</t>
+    <t>[default is yes] (yes or no)</t>
   </si>
   <si>
     <t>all sun compass info is optional</t>
@@ -86,7 +86,7 @@
     <t>bedding_dip</t>
   </si>
   <si>
-    <t>use_uncorrected_bedding</t>
+    <t>correct_bedding_using_local_dec</t>
   </si>
   <si>
     <t>shadow_angle</t>
@@ -354,7 +354,7 @@
   <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -579,7 +579,7 @@
       <c r="G7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="8" t="s">

</xml_diff>